<commit_message>
With fixes across the board. Able to run 2 iters with sim1 but not 3
</commit_message>
<xml_diff>
--- a/CGE/1model.xlsx
+++ b/CGE/1model.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF33232-5FC3-4EB7-88E1-4681E3649F7E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703F99E6-4F78-4EB5-A967-4507DD2CBF11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="905" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -6244,12 +6246,12 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D21" sqref="D21"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6257,107 +6259,121 @@
     <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>52325.432882070083</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>47</v>
       </c>
       <c r="B8">
-        <v>5303.2</v>
+        <f>L3/10</f>
+        <v>5232.5432882070081</v>
       </c>
       <c r="C8" s="11"/>
       <c r="I8" s="24"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>48</v>
       </c>
       <c r="B9">
-        <v>5303.2</v>
+        <f>B8</f>
+        <v>5232.5432882070081</v>
       </c>
       <c r="C9" s="11"/>
       <c r="I9" s="24"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>49</v>
       </c>
       <c r="B10" s="75">
-        <v>5303.2</v>
+        <f t="shared" ref="B10:B17" si="0">B9</f>
+        <v>5232.5432882070081</v>
       </c>
       <c r="C10" s="11"/>
       <c r="I10" s="24"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>50</v>
       </c>
       <c r="B11" s="75">
-        <v>5303.2</v>
+        <f t="shared" si="0"/>
+        <v>5232.5432882070081</v>
       </c>
       <c r="C11" s="11"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
       <c r="B12" s="75">
-        <v>5303.2</v>
+        <f t="shared" si="0"/>
+        <v>5232.5432882070081</v>
       </c>
       <c r="C12" s="11"/>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>52</v>
       </c>
       <c r="B13" s="75">
-        <v>5303.2</v>
+        <f t="shared" si="0"/>
+        <v>5232.5432882070081</v>
       </c>
       <c r="C13" s="11"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>53</v>
       </c>
       <c r="B14" s="75">
-        <v>5303.2</v>
+        <f t="shared" si="0"/>
+        <v>5232.5432882070081</v>
       </c>
       <c r="C14" s="11"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>54</v>
       </c>
       <c r="B15" s="75">
-        <v>5303.2</v>
+        <f t="shared" si="0"/>
+        <v>5232.5432882070081</v>
       </c>
       <c r="C15" s="11"/>
       <c r="I15" s="24"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>55</v>
       </c>
       <c r="B16" s="75">
-        <v>5303.2</v>
+        <f t="shared" si="0"/>
+        <v>5232.5432882070081</v>
       </c>
       <c r="C16" s="11"/>
       <c r="I16" s="24"/>
@@ -6367,7 +6383,8 @@
         <v>739</v>
       </c>
       <c r="B17" s="75">
-        <v>5303.2</v>
+        <f t="shared" si="0"/>
+        <v>5232.5432882070081</v>
       </c>
       <c r="C17" s="11"/>
     </row>

</xml_diff>

<commit_message>
small tweaks: CGE links, capacity reporting, IIS limits, CCS, agri model
</commit_message>
<xml_diff>
--- a/CGE/1model.xlsx
+++ b/CGE/1model.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C127D55A-980C-41F7-A944-197943E6499D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A96302-3D00-4457-9153-A278513C73EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="905" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4275" yWindow="-17430" windowWidth="28770" windowHeight="15570" tabRatio="905" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -118,7 +118,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
+    <author>tc={C7AEE201-4D85-4D0F-8941-FF043E24C344}</author>
     <author>tc={F2825210-4950-456F-8849-015930D0B032}</author>
+    <author>tc={CEAAEFF7-AA04-468B-BF7E-ADB4DBB607B6}</author>
   </authors>
   <commentList>
     <comment ref="M7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
@@ -145,7 +147,23 @@
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="1" shapeId="0" xr:uid="{F2825210-4950-456F-8849-015930D0B032}">
+    <comment ref="B16" authorId="1" shapeId="0" xr:uid="{C7AEE201-4D85-4D0F-8941-FF043E24C344}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Changed from 0.39 to allow for faster ramp up of gas imports</t>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="2" shapeId="0" xr:uid="{F2825210-4950-456F-8849-015930D0B032}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Changed from 0.39 to allow for faster ramp up of gas imports</t>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="3" shapeId="0" xr:uid="{CEAAEFF7-AA04-468B-BF7E-ADB4DBB607B6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -3104,10 +3122,6 @@
 </externalLink>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3429,7 +3443,13 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B16" dT="2021-09-27T08:56:01.52" personId="{00000000-0000-0000-0000-000000000000}" id="{C7AEE201-4D85-4D0F-8941-FF043E24C344}">
+    <text>Changed from 0.39 to allow for faster ramp up of gas imports</text>
+  </threadedComment>
   <threadedComment ref="B17" dT="2021-09-27T08:56:01.52" personId="{00000000-0000-0000-0000-000000000000}" id="{F2825210-4950-456F-8849-015930D0B032}">
+    <text>Changed from 0.39 to allow for faster ramp up of gas imports</text>
+  </threadedComment>
+  <threadedComment ref="B18" dT="2021-09-27T08:56:01.52" personId="{00000000-0000-0000-0000-000000000000}" id="{CEAAEFF7-AA04-468B-BF7E-ADB4DBB607B6}">
     <text>Changed from 0.39 to allow for faster ramp up of gas imports</text>
   </threadedComment>
 </ThreadedComments>
@@ -51320,7 +51340,7 @@
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D21" sqref="D21"/>
-      <selection pane="bottomLeft" activeCell="P20" sqref="P20"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51842,13 +51862,11 @@
         <f>Demand!A16</f>
         <v>ccoil</v>
       </c>
-      <c r="B16" s="22">
-        <f>VLOOKUP(VLOOKUP($A16,Elasticities_RawData!$N$8:$O$66,2,),Elasticities_RawData!$E$8:$G$48,2,)</f>
-        <v>0.38600000000000001</v>
-      </c>
-      <c r="C16" s="22">
-        <f>VLOOKUP(VLOOKUP($A16,Elasticities_RawData!$N$8:$O$66,2,),Elasticities_RawData!$E$8:$G$48,2,)</f>
-        <v>0.38600000000000001</v>
+      <c r="B16" s="72">
+        <v>0.74</v>
+      </c>
+      <c r="C16" s="72">
+        <v>0.74</v>
       </c>
       <c r="D16" s="11">
         <f t="shared" si="1"/>
@@ -51934,13 +51952,11 @@
         <f>Demand!A18</f>
         <v>chydr</v>
       </c>
-      <c r="B18" s="22">
-        <f>VLOOKUP(VLOOKUP($A18,Elasticities_RawData!$N$8:$O$66,2,),Elasticities_RawData!$E$8:$G$48,2,)</f>
-        <v>0.38600000000000001</v>
-      </c>
-      <c r="C18" s="22">
-        <f>VLOOKUP(VLOOKUP($A18,Elasticities_RawData!$N$8:$O$66,2,),Elasticities_RawData!$E$8:$G$48,2,)</f>
-        <v>0.38600000000000001</v>
+      <c r="B18" s="72">
+        <v>0.74</v>
+      </c>
+      <c r="C18" s="72">
+        <v>0.74</v>
       </c>
       <c r="D18" s="11">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Preliminary upgrades on H2 links in SATIM and CGE
</commit_message>
<xml_diff>
--- a/CGE/1model.xlsx
+++ b/CGE/1model.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A96302-3D00-4457-9153-A278513C73EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA3D9CF-5891-4EF1-BB7B-DCB1D4E7BEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="-17430" windowWidth="28770" windowHeight="15570" tabRatio="905" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="905" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -3457,6 +3457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V88"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -5159,7 +5160,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23AFCDF-769B-4D79-B62D-C5A6F52B7628}">
-  <sheetPr>
+  <sheetPr codeName="Sheet10">
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
   <dimension ref="A2:R43"/>
@@ -5874,6 +5875,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A2:E43"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -6115,6 +6117,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -6191,6 +6194,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -6338,6 +6342,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:AG66"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -10010,6 +10015,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:O103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11530,6 +11536,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F82"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -12356,6 +12363,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AX176"/>
   <sheetViews>
     <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -15411,6 +15419,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AT66"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -16343,14 +16352,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BCBF0E9-6DC9-429A-AB79-5F8256D1D190}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:ER154"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="DO56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection activeCell="G10" sqref="G10"/>
       <selection pane="topRight" activeCell="G10" sqref="G10"/>
       <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
-      <selection pane="bottomRight" activeCell="EQ72" sqref="EQ72"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7:ER154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18657,7 +18667,7 @@
       <c r="BI13" s="87"/>
       <c r="BJ13" s="87"/>
       <c r="BK13" s="87">
-        <v>98199.69575640859</v>
+        <v>89476.206652745168</v>
       </c>
       <c r="BL13" s="87"/>
       <c r="BM13" s="87"/>
@@ -18744,7 +18754,7 @@
       <c r="EP13" s="87"/>
       <c r="EQ13" s="87"/>
       <c r="ER13" s="87">
-        <v>98199.69575640859</v>
+        <v>89476.206652745168</v>
       </c>
     </row>
     <row r="14" spans="1:148" x14ac:dyDescent="0.25">
@@ -18814,7 +18824,7 @@
       <c r="BJ14" s="87"/>
       <c r="BK14" s="87"/>
       <c r="BL14" s="87">
-        <v>107795.80717375339</v>
+        <v>116519.29627741681</v>
       </c>
       <c r="BM14" s="87">
         <v>20022.292323937541</v>
@@ -18902,7 +18912,7 @@
       <c r="EP14" s="87"/>
       <c r="EQ14" s="87"/>
       <c r="ER14" s="87">
-        <v>127818.09949769093</v>
+        <v>136541.58860135436</v>
       </c>
     </row>
     <row r="15" spans="1:148" x14ac:dyDescent="0.25">
@@ -26658,13 +26668,13 @@
         <v>134.4266717394338</v>
       </c>
       <c r="AH64" s="87">
-        <v>3.5133854383545305E-4</v>
+        <v>2.7301509541168261E-4</v>
       </c>
       <c r="AI64" s="87">
-        <v>1.6036506325483471E-3</v>
+        <v>1.2822711803486973E-3</v>
       </c>
       <c r="AJ64" s="87">
-        <v>86.1123478584515</v>
+        <v>86.112747561352123</v>
       </c>
       <c r="AK64" s="87">
         <v>12.278975385051188</v>
@@ -27492,13 +27502,13 @@
         <v>112.9473647089075</v>
       </c>
       <c r="AH68" s="87">
-        <v>2.5269577430749946E-4</v>
+        <v>1.9636263126599011E-4</v>
       </c>
       <c r="AI68" s="87">
-        <v>1.1534052993067141E-3</v>
+        <v>9.2225722021025943E-4</v>
       </c>
       <c r="AJ68" s="87">
-        <v>61.935210185252863</v>
+        <v>61.935497666475001</v>
       </c>
       <c r="AK68" s="87">
         <v>15.643469439310474</v>
@@ -27673,13 +27683,13 @@
       <c r="G69" s="89"/>
       <c r="H69" s="89"/>
       <c r="I69" s="89">
-        <v>0.13647386580237011</v>
+        <v>0.16863043331290395</v>
       </c>
       <c r="J69" s="89">
-        <v>8.9527808404686587E-3</v>
+        <v>1.1062274110927072E-2</v>
       </c>
       <c r="K69" s="89">
-        <v>9.9330278017672573E-3</v>
+        <v>1.227349113673341E-2</v>
       </c>
       <c r="L69" s="89"/>
       <c r="M69" s="89"/>
@@ -27688,58 +27698,46 @@
       <c r="P69" s="89"/>
       <c r="Q69" s="89"/>
       <c r="R69" s="89"/>
-      <c r="S69" s="89">
-        <v>8.2056034095653576</v>
-      </c>
+      <c r="S69" s="89"/>
       <c r="T69" s="89"/>
-      <c r="U69" s="89">
-        <v>0.27742686995506127</v>
-      </c>
-      <c r="V69" s="89">
-        <v>6.3661047750047652</v>
-      </c>
+      <c r="U69" s="89"/>
+      <c r="V69" s="89"/>
       <c r="W69" s="89"/>
       <c r="X69" s="89"/>
       <c r="Y69" s="89"/>
       <c r="Z69" s="89"/>
       <c r="AA69" s="89"/>
       <c r="AB69" s="89"/>
-      <c r="AC69" s="89">
-        <v>0.15659213524581297</v>
-      </c>
-      <c r="AD69" s="89">
-        <v>25388.785202557039</v>
-      </c>
+      <c r="AC69" s="89"/>
+      <c r="AD69" s="89"/>
       <c r="AE69" s="89">
-        <v>6899.5131833250034</v>
-      </c>
-      <c r="AF69" s="89">
-        <v>1584.0307774392547</v>
-      </c>
+        <v>4274.432897734725</v>
+      </c>
+      <c r="AF69" s="89"/>
       <c r="AG69" s="89">
-        <v>1375.3992289763646</v>
+        <v>1438.8338445568154</v>
       </c>
       <c r="AH69" s="89">
-        <v>6.2569663358519765E-3</v>
+        <v>4.8621089007824846E-3</v>
       </c>
       <c r="AI69" s="89">
-        <v>2.8559314650720712E-2</v>
+        <v>2.2835887919637282E-2</v>
       </c>
       <c r="AJ69" s="89">
-        <v>1506.0335852119708</v>
+        <v>1382.6933187950401</v>
       </c>
       <c r="AK69" s="89">
-        <v>398.03513872028998</v>
+        <v>386.45403777148385</v>
       </c>
       <c r="AL69" s="89">
-        <v>2254.165961371396</v>
+        <v>2679.8650630972984</v>
       </c>
       <c r="AM69" s="89">
-        <v>193.90557684901427</v>
+        <v>192.49788475142279</v>
       </c>
       <c r="AN69" s="89"/>
       <c r="AO69" s="89">
-        <v>165.5692319429437</v>
+        <v>125.08000859574234</v>
       </c>
       <c r="AP69" s="89"/>
       <c r="AQ69" s="89"/>
@@ -27755,11 +27753,11 @@
       <c r="BA69" s="89"/>
       <c r="BB69" s="89"/>
       <c r="BC69" s="89">
-        <v>802.69388925901012</v>
+        <v>620.15805643867645</v>
       </c>
       <c r="BD69" s="89"/>
       <c r="BE69" s="89">
-        <v>5.2201037594586435</v>
+        <v>4.0330310784632184</v>
       </c>
       <c r="BF69" s="89"/>
       <c r="BG69" s="89"/>
@@ -27850,13 +27848,13 @@
       <c r="EN69" s="89"/>
       <c r="EO69" s="89"/>
       <c r="EP69" s="89">
-        <v>110.48702985183937</v>
+        <v>23091.945986038769</v>
       </c>
       <c r="EQ69" s="89">
-        <v>58319.278859883379</v>
+        <v>56098.388979367926</v>
       </c>
       <c r="ER69" s="89">
-        <v>99018.313672292163</v>
+        <v>90294.602772421742</v>
       </c>
     </row>
     <row r="70" spans="1:148" x14ac:dyDescent="0.25">
@@ -27871,13 +27869,13 @@
       <c r="G70" s="87"/>
       <c r="H70" s="87"/>
       <c r="I70" s="87">
-        <v>3.2157644462681406E-2</v>
+        <v>1.0769521475717525E-6</v>
       </c>
       <c r="J70" s="87">
-        <v>2.1095639192708886E-3</v>
+        <v>7.0648812475551659E-8</v>
       </c>
       <c r="K70" s="87">
-        <v>2.3405417191722424E-3</v>
+        <v>7.8384206089396335E-8</v>
       </c>
       <c r="L70" s="87"/>
       <c r="M70" s="87"/>
@@ -27887,14 +27885,14 @@
       <c r="Q70" s="87"/>
       <c r="R70" s="87"/>
       <c r="S70" s="87">
-        <v>1.9335048179018202</v>
+        <v>10.139108227467178</v>
       </c>
       <c r="T70" s="87"/>
       <c r="U70" s="87">
-        <v>6.5370718385955484E-2</v>
+        <v>0.34279758834101676</v>
       </c>
       <c r="V70" s="87">
-        <v>1.5000596104109656</v>
+        <v>7.8661643854157308</v>
       </c>
       <c r="W70" s="87"/>
       <c r="X70" s="87"/>
@@ -27903,41 +27901,41 @@
       <c r="AA70" s="87"/>
       <c r="AB70" s="87"/>
       <c r="AC70" s="87">
-        <v>3.6898157616339217E-2</v>
+        <v>0.19349029286215219</v>
       </c>
       <c r="AD70" s="87">
-        <v>5982.4166559883379</v>
+        <v>31371.201858545377</v>
       </c>
       <c r="AE70" s="87">
-        <v>1625.7478353858987</v>
+        <v>4250.8281209761772</v>
       </c>
       <c r="AF70" s="87">
-        <v>373.24874077064328</v>
+        <v>1957.279518209898</v>
       </c>
       <c r="AG70" s="87">
-        <v>324.08841897772322</v>
+        <v>260.65380339727244</v>
       </c>
       <c r="AH70" s="87">
-        <v>1.3355273399394104E-3</v>
+        <v>1.0377999525985275E-3</v>
       </c>
       <c r="AI70" s="87">
-        <v>6.0958847273030938E-3</v>
+        <v>4.8742395294212437E-3</v>
       </c>
       <c r="AJ70" s="87">
-        <v>354.87085907194387</v>
+        <v>478.21976314562573</v>
       </c>
       <c r="AK70" s="87">
-        <v>93.789916474974405</v>
+        <v>105.37101742378053</v>
       </c>
       <c r="AL70" s="87">
-        <v>531.15420391646103</v>
+        <v>105.45510219055859</v>
       </c>
       <c r="AM70" s="87">
-        <v>45.690407925217983</v>
+        <v>47.098100022809462</v>
       </c>
       <c r="AN70" s="87"/>
       <c r="AO70" s="87">
-        <v>39.013451135696897</v>
+        <v>79.502674482898257</v>
       </c>
       <c r="AP70" s="87"/>
       <c r="AQ70" s="87"/>
@@ -27953,11 +27951,11 @@
       <c r="BA70" s="87"/>
       <c r="BB70" s="87"/>
       <c r="BC70" s="87">
-        <v>189.14056952514295</v>
+        <v>371.67640234547662</v>
       </c>
       <c r="BD70" s="87"/>
       <c r="BE70" s="87">
-        <v>1.2300248092778983</v>
+        <v>2.4170974902733233</v>
       </c>
       <c r="BF70" s="87"/>
       <c r="BG70" s="87"/>
@@ -28048,13 +28046,13 @@
       <c r="EN70" s="87"/>
       <c r="EO70" s="87"/>
       <c r="EP70" s="87">
-        <v>1547.1541326586262</v>
+        <v>-21434.304823528302</v>
       </c>
       <c r="EQ70" s="87">
-        <v>184374.48243414148</v>
+        <v>186595.37231465691</v>
       </c>
       <c r="ER70" s="87">
-        <v>195485.60752324792</v>
+        <v>204209.31842311833</v>
       </c>
     </row>
     <row r="71" spans="1:148" x14ac:dyDescent="0.25">
@@ -28492,11 +28490,9 @@
       <c r="F73" s="87">
         <v>2.4884898400794748</v>
       </c>
-      <c r="G73" s="87">
-        <v>8.5743490567291705</v>
-      </c>
+      <c r="G73" s="87"/>
       <c r="H73" s="87">
-        <v>8.5743490567291705</v>
+        <v>17.148698113458341</v>
       </c>
       <c r="I73" s="87">
         <v>4.7783449873560997</v>
@@ -29161,10 +29157,10 @@
         <v>31.42222042311074</v>
       </c>
       <c r="G76" s="87">
-        <v>57.004897121621234</v>
+        <v>100.48152332291113</v>
       </c>
       <c r="H76" s="87">
-        <v>85.507345682431833</v>
+        <v>42.030719481141944</v>
       </c>
       <c r="I76" s="87">
         <v>153.99670260254308</v>
@@ -29448,13 +29444,13 @@
         <v>49.747835891863119</v>
       </c>
       <c r="AH77" s="87">
-        <v>4.73809533916335E-5</v>
+        <v>3.681837856358754E-5</v>
       </c>
       <c r="AI77" s="87">
-        <v>2.1626575623545215E-4</v>
+        <v>1.7292503796563461E-4</v>
       </c>
       <c r="AJ77" s="87">
-        <v>11.612973102774555</v>
+        <v>11.613027006067654</v>
       </c>
       <c r="AK77" s="87"/>
       <c r="AL77" s="87">
@@ -29643,10 +29639,10 @@
         <v>114.87566226637986</v>
       </c>
       <c r="G78" s="87">
-        <v>166.34010758723144</v>
+        <v>349.02527732911034</v>
       </c>
       <c r="H78" s="87">
-        <v>665.36043034892577</v>
+        <v>482.67526060704682</v>
       </c>
       <c r="I78" s="87">
         <v>184.55395449324314</v>
@@ -29698,13 +29694,13 @@
         <v>109.10050590892386</v>
       </c>
       <c r="AH78" s="87">
-        <v>1.5435555045210521E-4</v>
+        <v>1.199452666762942E-4</v>
       </c>
       <c r="AI78" s="87">
-        <v>7.0454090637945177E-4</v>
+        <v>5.6334745317408426E-4</v>
       </c>
       <c r="AJ78" s="87">
-        <v>37.832225545139373</v>
+        <v>37.83240114887635</v>
       </c>
       <c r="AK78" s="87">
         <v>136.0748104760799</v>
@@ -29884,7 +29880,7 @@
         <v>5675.8936556490207</v>
       </c>
       <c r="ER78" s="87">
-        <v>109403.70373058437</v>
+        <v>109403.70373058438</v>
       </c>
     </row>
     <row r="79" spans="1:148" x14ac:dyDescent="0.25">
@@ -29901,10 +29897,10 @@
         <v>17.135111156596562</v>
       </c>
       <c r="G79" s="87">
-        <v>39.850937792223853</v>
+        <v>43.068407461545974</v>
       </c>
       <c r="H79" s="87">
-        <v>92.985521515188992</v>
+        <v>89.768051845866864</v>
       </c>
       <c r="I79" s="87">
         <v>21.867793897141102</v>
@@ -30123,10 +30119,10 @@
         <v>115.83218322780114</v>
       </c>
       <c r="G80" s="87">
-        <v>162.13057678768126</v>
+        <v>211.96269286421307</v>
       </c>
       <c r="H80" s="87">
-        <v>648.52230715072506</v>
+        <v>598.69019107419319</v>
       </c>
       <c r="I80" s="87">
         <v>146.99871021152131</v>
@@ -30341,10 +30337,10 @@
         <v>131.83310646223114</v>
       </c>
       <c r="G81" s="87">
-        <v>438.97153173659592</v>
+        <v>431.07570605065513</v>
       </c>
       <c r="H81" s="87">
-        <v>536.52076101139494</v>
+        <v>544.41658669733579</v>
       </c>
       <c r="I81" s="87">
         <v>795.1415561027635</v>
@@ -30422,13 +30418,13 @@
         <v>239.53317204334533</v>
       </c>
       <c r="AH81" s="87">
-        <v>3.3394427901633984E-4</v>
+        <v>2.5949851161371942E-4</v>
       </c>
       <c r="AI81" s="87">
-        <v>1.524256201537816E-3</v>
+        <v>1.2187877827191218E-3</v>
       </c>
       <c r="AJ81" s="87">
-        <v>81.849049827911486</v>
+        <v>81.849429742097712</v>
       </c>
       <c r="AK81" s="87">
         <v>123.66527191772326</v>
@@ -30604,7 +30600,7 @@
         <v>5029.9800896295146</v>
       </c>
       <c r="ER81" s="87">
-        <v>59771.082006278797</v>
+        <v>59771.082006278804</v>
       </c>
     </row>
     <row r="82" spans="1:148" x14ac:dyDescent="0.25">
@@ -30627,10 +30623,10 @@
         <v>29.082420698480046</v>
       </c>
       <c r="G82" s="87">
-        <v>105.46583206845051</v>
+        <v>105.54543828890147</v>
       </c>
       <c r="H82" s="87">
-        <v>130.99966509554906</v>
+        <v>130.92005887509811</v>
       </c>
       <c r="I82" s="87">
         <v>59.723949437851502</v>
@@ -30708,13 +30704,13 @@
         <v>226.87822649637727</v>
       </c>
       <c r="AH82" s="87">
-        <v>5.7754117020765796E-4</v>
+        <v>4.4879066204095647E-4</v>
       </c>
       <c r="AI82" s="87">
-        <v>2.6361305332898246E-3</v>
+        <v>2.1078370449698785E-3</v>
       </c>
       <c r="AJ82" s="87">
-        <v>141.55414189630511</v>
+        <v>141.55479894030159</v>
       </c>
       <c r="AK82" s="87">
         <v>81.849726550251688</v>
@@ -30915,10 +30911,10 @@
         <v>4.5944133584144931</v>
       </c>
       <c r="G83" s="87">
-        <v>20.376575712575058</v>
+        <v>26.747975978840866</v>
       </c>
       <c r="H83" s="87">
-        <v>11.320319840319474</v>
+        <v>4.9489195740536651</v>
       </c>
       <c r="I83" s="87">
         <v>5.4446201488513628</v>
@@ -30996,13 +30992,13 @@
         <v>37.291698418022172</v>
       </c>
       <c r="AH83" s="87">
-        <v>7.0606253111179363E-5</v>
+        <v>5.4866092172449184E-5</v>
       </c>
       <c r="AI83" s="87">
-        <v>3.2227537926109498E-4</v>
+        <v>2.5768981259076688E-4</v>
       </c>
       <c r="AJ83" s="87">
-        <v>17.305445961211184</v>
+        <v>17.305526286938793</v>
       </c>
       <c r="AK83" s="87">
         <v>1891.2989719572008</v>
@@ -31369,10 +31365,10 @@
         <v>1085.7639893589812</v>
       </c>
       <c r="G85" s="87">
-        <v>1946.7191209604866</v>
+        <v>3328.4798766251083</v>
       </c>
       <c r="H85" s="87">
-        <v>5693.0754858782038</v>
+        <v>4311.3147302135822</v>
       </c>
       <c r="I85" s="87">
         <v>1178.5522850351588</v>
@@ -31797,10 +31793,10 @@
         <v>37.137901005427636</v>
       </c>
       <c r="G87" s="87">
-        <v>137.97790380493788</v>
+        <v>228.23859926064705</v>
       </c>
       <c r="H87" s="87">
-        <v>121.76624512893653</v>
+        <v>31.505549673227378</v>
       </c>
       <c r="I87" s="87">
         <v>57.965793718524559</v>
@@ -31876,13 +31872,13 @@
         <v>97.60497265252998</v>
       </c>
       <c r="AH87" s="87">
-        <v>5.380086350736873E-4</v>
+        <v>4.1807106397567415E-4</v>
       </c>
       <c r="AI87" s="87">
-        <v>2.4556881193099822E-3</v>
+        <v>1.9635561757688214E-3</v>
       </c>
       <c r="AJ87" s="87">
-        <v>131.86479998133916</v>
+        <v>131.86541205085379</v>
       </c>
       <c r="AK87" s="87">
         <v>35.117769436752816</v>
@@ -32058,7 +32054,7 @@
         <v>3926.8027590883289</v>
       </c>
       <c r="ER87" s="87">
-        <v>20893.067988578747</v>
+        <v>20893.06798857875</v>
       </c>
     </row>
     <row r="88" spans="1:148" x14ac:dyDescent="0.25">
@@ -32081,10 +32077,10 @@
         <v>334.16418597192558</v>
       </c>
       <c r="G88" s="87">
-        <v>1241.8011342444406</v>
+        <v>2054.1473933458228</v>
       </c>
       <c r="H88" s="87">
-        <v>1095.8192830835053</v>
+        <v>283.47302398212321</v>
       </c>
       <c r="I88" s="87">
         <v>521.61522038979774</v>
@@ -32162,13 +32158,13 @@
         <v>878.36783079584632</v>
       </c>
       <c r="AH88" s="87">
-        <v>4.8420777156631843E-3</v>
+        <v>3.7626395757810664E-3</v>
       </c>
       <c r="AI88" s="87">
-        <v>2.2101193073789833E-2</v>
+        <v>1.7672005581919385E-2</v>
       </c>
       <c r="AJ88" s="87">
-        <v>1186.7831998320521</v>
+        <v>1186.7887084576837</v>
       </c>
       <c r="AK88" s="87">
         <v>316.05992493077525</v>
@@ -32367,10 +32363,10 @@
         <v>1266.7562210538081</v>
       </c>
       <c r="G89" s="87">
-        <v>3808.3976130068436</v>
+        <v>1423.7755003399416</v>
       </c>
       <c r="H89" s="87">
-        <v>5110.5663518803776</v>
+        <v>7495.1884645472801</v>
       </c>
       <c r="I89" s="87">
         <v>1687.9808356221197</v>
@@ -32448,13 +32444,13 @@
         <v>306.62203769326663</v>
       </c>
       <c r="AH89" s="87">
-        <v>1.3045896653131259E-3</v>
+        <v>1.0137591738735307E-3</v>
       </c>
       <c r="AI89" s="87">
-        <v>5.9546727186734569E-3</v>
+        <v>4.7613270999245548E-3</v>
       </c>
       <c r="AJ89" s="87">
-        <v>319.75221934936911</v>
+        <v>319.75370352547935</v>
       </c>
       <c r="AK89" s="87">
         <v>73.286500758557636</v>
@@ -32655,10 +32651,10 @@
         <v>390.60157780444706</v>
       </c>
       <c r="G90" s="87">
-        <v>1477.1036284499357</v>
+        <v>1123.7909905055421</v>
       </c>
       <c r="H90" s="87">
-        <v>1238.6207015558996</v>
+        <v>1591.9333395002932</v>
       </c>
       <c r="I90" s="87">
         <v>452.89314867551178</v>
@@ -32724,13 +32720,13 @@
         <v>420.79139053936831</v>
       </c>
       <c r="AH90" s="87">
-        <v>2.268130909578437E-5</v>
+        <v>1.7624994113220816E-5</v>
       </c>
       <c r="AI90" s="87">
-        <v>1.0352663070042828E-4</v>
+        <v>8.2779386140241311E-5</v>
       </c>
       <c r="AJ90" s="87">
-        <v>5.5591418365135858</v>
+        <v>5.5591676400731282</v>
       </c>
       <c r="AK90" s="87">
         <v>63.423578945224413</v>
@@ -32931,10 +32927,10 @@
         <v>122.17730358587094</v>
       </c>
       <c r="G91" s="87">
-        <v>486.04007759991839</v>
+        <v>287.51952967497772</v>
       </c>
       <c r="H91" s="87">
-        <v>667.71525223678111</v>
+        <v>866.23580016172173</v>
       </c>
       <c r="I91" s="87">
         <v>238.41446200055714</v>
@@ -33012,13 +33008,13 @@
         <v>659.86233853128999</v>
       </c>
       <c r="AH91" s="87">
-        <v>6.169797242234037E-3</v>
+        <v>4.7943723007748363E-3</v>
       </c>
       <c r="AI91" s="87">
-        <v>2.8161439795906764E-2</v>
+        <v>2.2517749137187754E-2</v>
       </c>
       <c r="AJ91" s="87">
-        <v>1512.2045010318311</v>
+        <v>1512.2115201474312</v>
       </c>
       <c r="AK91" s="87">
         <v>493.5729614559516</v>
@@ -33217,10 +33213,10 @@
         <v>13.008886383115954</v>
       </c>
       <c r="G92" s="87">
-        <v>48.031361560409657</v>
+        <v>31.452818587755644</v>
       </c>
       <c r="H92" s="87">
-        <v>64.041815413879561</v>
+        <v>80.620358386533567</v>
       </c>
       <c r="I92" s="87">
         <v>20.15355576569408</v>
@@ -33290,13 +33286,13 @@
         <v>134.95058421086716</v>
       </c>
       <c r="AH92" s="87">
-        <v>3.2287133179567646E-4</v>
+        <v>2.5089404223516533E-4</v>
       </c>
       <c r="AI92" s="87">
-        <v>1.4737148102610658E-3</v>
+        <v>1.1783751341449631E-3</v>
       </c>
       <c r="AJ92" s="87">
-        <v>79.135093071816925</v>
+        <v>79.13546038878259</v>
       </c>
       <c r="AK92" s="87">
         <v>264.62595755535926</v>
@@ -33499,10 +33495,10 @@
         <v>69.078520790903525</v>
       </c>
       <c r="G93" s="87">
-        <v>263.74467764510007</v>
+        <v>203.26645454484563</v>
       </c>
       <c r="H93" s="87">
-        <v>229.8556967186347</v>
+        <v>290.33391981888917</v>
       </c>
       <c r="I93" s="87">
         <v>214.91617422751767</v>
@@ -33562,13 +33558,13 @@
         <v>75.138403425486842</v>
       </c>
       <c r="AH93" s="87">
-        <v>1.6091421677284139E-4</v>
+        <v>1.2504181797346072E-4</v>
       </c>
       <c r="AI93" s="87">
-        <v>7.3447730128535212E-4</v>
+        <v>5.8728444771158773E-4</v>
       </c>
       <c r="AJ93" s="87">
-        <v>39.439740598813245</v>
+        <v>39.439923664065617</v>
       </c>
       <c r="AK93" s="87"/>
       <c r="AL93" s="87">
@@ -33769,10 +33765,10 @@
         <v>156.82225666015532</v>
       </c>
       <c r="G94" s="87">
-        <v>600.53417757116654</v>
+        <v>603.90286938985014</v>
       </c>
       <c r="H94" s="87">
-        <v>497.28444177822917</v>
+        <v>493.91574995954556</v>
       </c>
       <c r="I94" s="87">
         <v>247.21965998197396</v>
@@ -33842,13 +33838,13 @@
         <v>15398.129405640264</v>
       </c>
       <c r="AH94" s="90">
-        <v>1.7252138466251205E-2</v>
+        <v>1.3406141489631358E-2</v>
       </c>
       <c r="AI94" s="87">
-        <v>7.8745709087849988E-2</v>
+        <v>6.2964682761990798E-2</v>
       </c>
       <c r="AJ94" s="87">
-        <v>4228.4633375419908</v>
+        <v>4228.4829645652944</v>
       </c>
       <c r="AK94" s="87">
         <v>364.94844162745812</v>
@@ -34021,10 +34017,10 @@
         <v>54.698484198590521</v>
       </c>
       <c r="G95" s="87">
-        <v>199.0609354641675</v>
+        <v>129.06374366714738</v>
       </c>
       <c r="H95" s="87">
-        <v>178.59672714542128</v>
+        <v>248.59391894244141</v>
       </c>
       <c r="I95" s="87">
         <v>112.84194260500111</v>
@@ -34092,13 +34088,13 @@
         <v>1537.3086077697074</v>
       </c>
       <c r="AH95" s="87">
-        <v>3.5387705473923059E-2</v>
+        <v>2.7498769935383083E-2</v>
       </c>
       <c r="AI95" s="87">
-        <v>0.16152374188204513</v>
+        <v>0.12915359178220767</v>
       </c>
       <c r="AJ95" s="87">
-        <v>8673.4531766843484</v>
+        <v>8673.4934357699858</v>
       </c>
       <c r="AK95" s="87">
         <v>155.12736876339807</v>
@@ -34273,10 +34269,10 @@
         <v>954.53967015139915</v>
       </c>
       <c r="G96" s="87">
-        <v>3671.9180540420793</v>
+        <v>4372.2135880061551</v>
       </c>
       <c r="H96" s="87">
-        <v>3038.33219373678</v>
+        <v>2338.0366597727043</v>
       </c>
       <c r="I96" s="87">
         <v>1653.2223999034443</v>
@@ -34348,13 +34344,13 @@
         <v>12460.129631715641</v>
       </c>
       <c r="AH96" s="87">
-        <v>7.6138218911347205E-3</v>
+        <v>5.9164823971868076E-3</v>
       </c>
       <c r="AI96" s="87">
-        <v>3.4752549943814513E-2</v>
+        <v>2.7787968483988748E-2</v>
       </c>
       <c r="AJ96" s="87">
-        <v>1866.1319454471352</v>
+        <v>1866.1406073680887</v>
       </c>
       <c r="AK96" s="87">
         <v>161.59785946708635</v>
@@ -34559,10 +34555,10 @@
         <v>1788.9213915428616</v>
       </c>
       <c r="G97" s="87">
-        <v>6175.8659349919071</v>
+        <v>2688.3543084615576</v>
       </c>
       <c r="H97" s="87">
-        <v>6427.9420956038211</v>
+        <v>9915.4537221341707</v>
       </c>
       <c r="I97" s="87">
         <v>2298.458976876107</v>
@@ -34624,13 +34620,13 @@
         <v>9247.0002502149091</v>
       </c>
       <c r="AH97" s="87">
-        <v>2.4921133553988336E-2</v>
+        <v>1.9365497393863923E-2</v>
       </c>
       <c r="AI97" s="87">
-        <v>0.11375009172461438</v>
+        <v>9.0954015432096622E-2</v>
       </c>
       <c r="AJ97" s="87">
-        <v>6108.1181187247139</v>
+        <v>6108.1464704371665</v>
       </c>
       <c r="AK97" s="87">
         <v>331.87918766876635</v>
@@ -35151,10 +35147,10 @@
         <v>300.31787040947808</v>
       </c>
       <c r="G100" s="87">
-        <v>1136.8577637092424</v>
+        <v>531.46064008705127</v>
       </c>
       <c r="H100" s="87">
-        <v>993.63158875374734</v>
+        <v>1599.0287123759385</v>
       </c>
       <c r="I100" s="87">
         <v>427.8402818614943</v>
@@ -35208,13 +35204,13 @@
         <v>3276.4440442386772</v>
       </c>
       <c r="AH100" s="87">
-        <v>9.8279722309513578E-3</v>
+        <v>7.6370350575404068E-3</v>
       </c>
       <c r="AI100" s="87">
-        <v>4.4858823950195789E-2</v>
+        <v>3.5868895611175344E-2</v>
       </c>
       <c r="AJ100" s="87">
-        <v>2408.815598843576</v>
+        <v>2408.8267797090884</v>
       </c>
       <c r="AK100" s="87">
         <v>5164.4423461763581</v>
@@ -35413,10 +35409,10 @@
         <v>97.775609549932668</v>
       </c>
       <c r="G101" s="87">
-        <v>391.66531222222261</v>
+        <v>76.848643184579117</v>
       </c>
       <c r="H101" s="87">
-        <v>293.74898416666701</v>
+        <v>608.56565320431048</v>
       </c>
       <c r="I101" s="87">
         <v>120.95146262453373</v>
@@ -35470,13 +35466,13 @@
         <v>9460.5138008332287</v>
       </c>
       <c r="AH101" s="87">
-        <v>3.4371753972098303E-2</v>
+        <v>2.6709303191494508E-2</v>
       </c>
       <c r="AI101" s="87">
-        <v>0.15688653000442446</v>
+        <v>0.12544569990902912</v>
       </c>
       <c r="AJ101" s="87">
-        <v>8424.4455715169534</v>
+        <v>8424.4846747978318</v>
       </c>
       <c r="AK101" s="87">
         <v>7732.6410198646527</v>
@@ -35677,10 +35673,10 @@
         <v>422.94140754763214</v>
       </c>
       <c r="G102" s="87">
-        <v>1371.4638362523012</v>
+        <v>895.2379007640435</v>
       </c>
       <c r="H102" s="87">
-        <v>2948.8895560407254</v>
+        <v>3425.1154915289831</v>
       </c>
       <c r="I102" s="87">
         <v>747.27216490603189</v>
@@ -35738,13 +35734,13 @@
         <v>1080.8530012081999</v>
       </c>
       <c r="AH102" s="87">
-        <v>6.1057993405787894E-3</v>
+        <v>4.7446413687916439E-3</v>
       </c>
       <c r="AI102" s="87">
-        <v>2.7869327594521678E-2</v>
+        <v>2.2284177653685087E-2</v>
       </c>
       <c r="AJ102" s="87">
-        <v>1496.5187481265609</v>
+        <v>1496.5256944344735</v>
       </c>
       <c r="AK102" s="87">
         <v>37.25366217003473</v>
@@ -35935,10 +35931,10 @@
         <v>26.975158213037613</v>
       </c>
       <c r="G103" s="87">
-        <v>97.48816050803525</v>
+        <v>46.447202216334922</v>
       </c>
       <c r="H103" s="87">
-        <v>91.579787143911901</v>
+        <v>142.62074543561224</v>
       </c>
       <c r="I103" s="87">
         <v>45.166513931102152</v>
@@ -35976,13 +35972,13 @@
         <v>219.33296274627122</v>
       </c>
       <c r="AH103" s="87">
-        <v>5.8887720548226477E-3</v>
+        <v>4.5759956959291722E-3</v>
       </c>
       <c r="AI103" s="87">
-        <v>2.6878727644161302E-2</v>
+        <v>2.149209879197974E-2</v>
       </c>
       <c r="AJ103" s="87">
-        <v>1443.3258101725985</v>
+        <v>1443.3325095778096</v>
       </c>
       <c r="AK103" s="87"/>
       <c r="AL103" s="87">
@@ -36169,10 +36165,10 @@
         <v>4.0823158174540106</v>
       </c>
       <c r="G104" s="87">
-        <v>21.845601133015478</v>
+        <v>17.837183040117996</v>
       </c>
       <c r="H104" s="87">
-        <v>8.9952475253593143</v>
+        <v>13.003665618256797</v>
       </c>
       <c r="I104" s="87">
         <v>5.2622327923772625</v>
@@ -36220,13 +36216,13 @@
         <v>5.8628892450465937</v>
       </c>
       <c r="AH104" s="87">
-        <v>7.421304795007165E-5</v>
+        <v>5.7668828889920539E-5</v>
       </c>
       <c r="AI104" s="87">
-        <v>3.3873824371575796E-4</v>
+        <v>2.7085343826318398E-4</v>
       </c>
       <c r="AJ104" s="87">
-        <v>18.189464175279969</v>
+        <v>18.189548604304481</v>
       </c>
       <c r="AK104" s="87">
         <v>7.8542020556095284</v>
@@ -36419,10 +36415,10 @@
         <v>2.1075631728626942</v>
       </c>
       <c r="G105" s="87">
-        <v>7.7414691796026549</v>
+        <v>7.2809434769719648</v>
       </c>
       <c r="H105" s="87">
-        <v>7.1393549100780049</v>
+        <v>7.5998806127086951</v>
       </c>
       <c r="I105" s="87">
         <v>3.8357948670471806</v>
@@ -36500,13 +36496,13 @@
         <v>203.874744569364</v>
       </c>
       <c r="AH105" s="87">
-        <v>3.7347570727092326E-4</v>
+        <v>2.9021724955480868E-4</v>
       </c>
       <c r="AI105" s="87">
-        <v>1.7046935632742861E-3</v>
+        <v>1.3630646121711584E-3</v>
       </c>
       <c r="AJ105" s="87">
-        <v>91.538120843224064</v>
+        <v>91.53854573063289</v>
       </c>
       <c r="AK105" s="87">
         <v>13.776145405355704</v>
@@ -36711,10 +36707,10 @@
         <v>12716.171521870787</v>
       </c>
       <c r="G106" s="87">
-        <v>16353.289368041114</v>
+        <v>6687.1427314889488</v>
       </c>
       <c r="H106" s="87">
-        <v>3608.6657443966997</v>
+        <v>7412.2023308162779</v>
       </c>
       <c r="I106" s="87">
         <v>1528.5186870108737</v>
@@ -36783,7 +36779,7 @@
         <v>7087.4319569537702</v>
       </c>
       <c r="AE106" s="87">
-        <v>6882.1944066773849</v>
+        <v>12744.804456809972</v>
       </c>
       <c r="AF106" s="87">
         <v>897.76803490422924</v>
@@ -36792,13 +36788,13 @@
         <v>894.24859579824147</v>
       </c>
       <c r="AH106" s="87">
-        <v>1.9941539980007704E-3</v>
+        <v>1.5495998192693327E-3</v>
       </c>
       <c r="AI106" s="87">
-        <v>9.1021220882342956E-3</v>
+        <v>7.2780121785075078E-3</v>
       </c>
       <c r="AJ106" s="87">
-        <v>488.76300704156256</v>
+        <v>488.76527570565099</v>
       </c>
       <c r="AK106" s="87">
         <v>161.07945874819038</v>
@@ -36997,10 +36993,10 @@
         <v>272.32956912457763</v>
       </c>
       <c r="G107" s="87">
-        <v>1799.5154653102184</v>
+        <v>2157.9318016464031</v>
       </c>
       <c r="H107" s="87">
-        <v>3173.4193890325432</v>
+        <v>2815.0030526963583</v>
       </c>
       <c r="I107" s="87">
         <v>414.49640921779587</v>
@@ -37078,13 +37074,13 @@
         <v>23.806819236026524</v>
       </c>
       <c r="AH107" s="87">
-        <v>9.3710089851590099E-5</v>
+        <v>7.281942038745237E-5</v>
       </c>
       <c r="AI107" s="87">
-        <v>4.2773059632491292E-4</v>
+        <v>3.4201128692802298E-4</v>
       </c>
       <c r="AJ107" s="87">
-        <v>22.968148876015849</v>
+        <v>22.96825548599471</v>
       </c>
       <c r="AK107" s="87">
         <v>7.8677376787724729</v>
@@ -37285,10 +37281,10 @@
         <v>58.923730117492497</v>
       </c>
       <c r="G108" s="87">
-        <v>110.61757989867907</v>
+        <v>96.148574784909812</v>
       </c>
       <c r="H108" s="87">
-        <v>85.891297333091998</v>
+        <v>100.36030244686125</v>
       </c>
       <c r="I108" s="87">
         <v>14.572976017166461</v>
@@ -37366,13 +37362,13 @@
         <v>39.663125647149656</v>
       </c>
       <c r="AH108" s="87">
-        <v>2.1278530248937258E-3</v>
+        <v>1.65349349454091E-3</v>
       </c>
       <c r="AI108" s="87">
-        <v>9.712378300682202E-3</v>
+        <v>7.7659700528527557E-3</v>
       </c>
       <c r="AJ108" s="87">
-        <v>521.53236097377805</v>
+        <v>521.53478174155623</v>
       </c>
       <c r="AK108" s="87">
         <v>10.632431755378299</v>
@@ -37577,10 +37573,10 @@
         <v>21.127108776419192</v>
       </c>
       <c r="G109" s="87">
-        <v>20.05168364884657</v>
+        <v>19.179859361217598</v>
       </c>
       <c r="H109" s="87">
-        <v>19.148196713058468</v>
+        <v>20.020021000687439</v>
       </c>
       <c r="I109" s="87">
         <v>6.8864932900587181</v>
@@ -37658,13 +37654,13 @@
         <v>48.608835000525673</v>
       </c>
       <c r="AH109" s="87">
-        <v>1.4503724165509872E-4</v>
+        <v>1.1270427644072889E-4</v>
       </c>
       <c r="AI109" s="87">
-        <v>6.6200839163322201E-4</v>
+        <v>5.2933866299253443E-4</v>
       </c>
       <c r="AJ109" s="87">
-        <v>35.548326743599276</v>
+        <v>35.548491746293138</v>
       </c>
       <c r="AK109" s="87">
         <v>11.535290712979663</v>
@@ -37843,10 +37839,10 @@
         <v>20.914929418186667</v>
       </c>
       <c r="G110" s="87">
-        <v>112.65985847666785</v>
+        <v>147.58347206794213</v>
       </c>
       <c r="H110" s="87">
-        <v>34.924556127767019</v>
+        <v>9.4253649274378404E-4</v>
       </c>
       <c r="I110" s="87">
         <v>24.901150172443412</v>
@@ -37924,13 +37920,13 @@
         <v>115.22894375126199</v>
       </c>
       <c r="AH110" s="87">
-        <v>2.9574888233360362E-4</v>
+        <v>2.2981796544936764E-4</v>
       </c>
       <c r="AI110" s="87">
-        <v>1.3499170260461797E-3</v>
+        <v>1.079387033078636E-3</v>
       </c>
       <c r="AJ110" s="87">
-        <v>72.487437780610023</v>
+        <v>72.487774241519887</v>
       </c>
       <c r="AK110" s="87">
         <v>38.209848574020953</v>
@@ -38309,10 +38305,10 @@
         <v>770.06313756549082</v>
       </c>
       <c r="G112" s="87">
-        <v>37.095432348875633</v>
+        <v>1865.5861706252063</v>
       </c>
       <c r="H112" s="87">
-        <v>2783.369848878885</v>
+        <v>954.87911060255419</v>
       </c>
       <c r="I112" s="87">
         <v>988.22703605036543</v>
@@ -38390,13 +38386,13 @@
         <v>902.26477621643085</v>
       </c>
       <c r="AH112" s="87">
-        <v>5.476721596824349E-3</v>
+        <v>4.2558031150732546E-3</v>
       </c>
       <c r="AI112" s="87">
-        <v>2.4997963380732572E-2</v>
+        <v>1.9988248911540336E-2</v>
       </c>
       <c r="AJ112" s="87">
-        <v>1342.3330978248835</v>
+        <v>1342.3393284578344</v>
       </c>
       <c r="AK112" s="87">
         <v>252.79185433652896</v>
@@ -38776,11 +38772,9 @@
       <c r="F114" s="87">
         <v>14.865004511114494</v>
       </c>
-      <c r="G114" s="87">
-        <v>1.3822858390287069E-2</v>
-      </c>
+      <c r="G114" s="87"/>
       <c r="H114" s="87">
-        <v>54.431361028011253</v>
+        <v>54.445183886401537</v>
       </c>
       <c r="I114" s="87">
         <v>19.076357031367003</v>
@@ -38858,13 +38852,13 @@
         <v>17.416974419888138</v>
       </c>
       <c r="AH114" s="87">
-        <v>1.0572053902585139E-4</v>
+        <v>8.2152395618270845E-5</v>
       </c>
       <c r="AI114" s="87">
-        <v>4.8255112414185083E-4</v>
+        <v>3.8584551209180364E-4</v>
       </c>
       <c r="AJ114" s="87">
-        <v>25.911885118504557</v>
+        <v>25.912005392260017</v>
       </c>
       <c r="AK114" s="87">
         <v>4.8797973461830839</v>
@@ -39061,10 +39055,10 @@
         <v>4250.4623080367328</v>
       </c>
       <c r="G115" s="87">
-        <v>831.77187670882267</v>
+        <v>1570.3715384816498</v>
       </c>
       <c r="H115" s="87">
-        <v>12523.805125622992</v>
+        <v>11785.205463850165</v>
       </c>
       <c r="I115" s="87">
         <v>5024.216232104136</v>
@@ -39142,13 +39136,13 @@
         <v>351.05654260126664</v>
       </c>
       <c r="AH115" s="87">
-        <v>9.2920419330795243E-4</v>
+        <v>7.2205790097347987E-4</v>
       </c>
       <c r="AI115" s="87">
-        <v>4.2412622199025259E-3</v>
+        <v>3.3912924688842966E-3</v>
       </c>
       <c r="AJ115" s="87">
-        <v>227.74601996383896</v>
+        <v>227.7470770798823</v>
       </c>
       <c r="AK115" s="87">
         <v>88.497143762957847</v>
@@ -39505,10 +39499,10 @@
         <v>14.213756080223684</v>
       </c>
       <c r="G117" s="87">
-        <v>25.5754090541548</v>
+        <v>18.085390414579599</v>
       </c>
       <c r="H117" s="87">
-        <v>11.387590892725857</v>
+        <v>18.877609532301058</v>
       </c>
       <c r="I117" s="87">
         <v>83.965137975883266</v>
@@ -39586,13 +39580,13 @@
         <v>106.09332231000194</v>
       </c>
       <c r="AH117" s="87">
-        <v>3.1451452705855441E-4</v>
+        <v>2.444002091995542E-4</v>
       </c>
       <c r="AI117" s="87">
-        <v>1.4355709873361171E-3</v>
+        <v>1.1478755204184607E-3</v>
       </c>
       <c r="AJ117" s="87">
-        <v>77.086857418543801</v>
+        <v>77.087215228328589</v>
       </c>
       <c r="AK117" s="87">
         <v>10569.09070536055</v>
@@ -39791,10 +39785,10 @@
         <v>457.74786775753444</v>
       </c>
       <c r="G118" s="87">
-        <v>5760.4315996179757</v>
+        <v>5458.1835878187303</v>
       </c>
       <c r="H118" s="87">
-        <v>1782.3488308750357</v>
+        <v>2084.5968426742811</v>
       </c>
       <c r="I118" s="87">
         <v>5911.395753730063</v>
@@ -39872,13 +39866,13 @@
         <v>1486.6942377522523</v>
       </c>
       <c r="AH118" s="87">
-        <v>2.0140149637300365E-3</v>
+        <v>1.5650332055250785E-3</v>
       </c>
       <c r="AI118" s="87">
-        <v>9.192775535781102E-3</v>
+        <v>7.3504982305373093E-3</v>
       </c>
       <c r="AJ118" s="87">
-        <v>493.6308884167251</v>
+        <v>493.63317967578854</v>
       </c>
       <c r="AK118" s="87">
         <v>674.66101456827732</v>
@@ -40079,10 +40073,10 @@
         <v>6381.7367639630102</v>
       </c>
       <c r="G119" s="87">
-        <v>4143.1586061590833</v>
+        <v>5205.8948088384095</v>
       </c>
       <c r="H119" s="87">
-        <v>1062.7694499377494</v>
+        <v>3.3247258423216408E-2</v>
       </c>
       <c r="I119" s="87">
         <v>877.77507003334722</v>
@@ -40160,13 +40154,13 @@
         <v>3391.0620437932594</v>
       </c>
       <c r="AH119" s="87">
-        <v>8.4024571961487503E-3</v>
+        <v>6.5293082508291718E-3</v>
       </c>
       <c r="AI119" s="87">
-        <v>3.8352199136668284E-2</v>
+        <v>3.0666230323368956E-2</v>
       </c>
       <c r="AJ119" s="87">
-        <v>2059.4248220662657</v>
+        <v>2059.4343811840245</v>
       </c>
       <c r="AK119" s="87">
         <v>1130.8329468686077</v>
@@ -40569,10 +40563,10 @@
         <v>1858.3874239891518</v>
       </c>
       <c r="G121" s="87">
-        <v>1117.2433838305315</v>
+        <v>905.81891399614358</v>
       </c>
       <c r="H121" s="87">
-        <v>734.07327024244296</v>
+        <v>945.49774007683084</v>
       </c>
       <c r="I121" s="87">
         <v>686.23032581991288</v>
@@ -40650,13 +40644,13 @@
         <v>1337.0060187436272</v>
       </c>
       <c r="AH121" s="87">
-        <v>8.5147159529900349E-3</v>
+        <v>6.6165413077982193E-3</v>
       </c>
       <c r="AI121" s="87">
-        <v>3.8864593320501212E-2</v>
+        <v>3.1075938199618274E-2</v>
       </c>
       <c r="AJ121" s="87">
-        <v>2086.9392102122442</v>
+        <v>2086.9488970420102</v>
       </c>
       <c r="AK121" s="87">
         <v>480.75147173077352</v>
@@ -41069,10 +41063,10 @@
         <v>5082.4614129361635</v>
       </c>
       <c r="BK123" s="87">
-        <v>96.524249756018719</v>
+        <v>96.498097491252238</v>
       </c>
       <c r="BL123" s="87">
-        <v>125.63731551530407</v>
+        <v>125.66346778007055</v>
       </c>
       <c r="BM123" s="87">
         <v>12882.07637076112</v>
@@ -41243,10 +41237,10 @@
         <v>2307.1530276613476</v>
       </c>
       <c r="G124" s="87">
-        <v>1897.0204877534902</v>
+        <v>1728.9576395197957</v>
       </c>
       <c r="H124" s="87">
-        <v>2852.2361085188381</v>
+        <v>3020.2989567525328</v>
       </c>
       <c r="I124" s="87">
         <v>295.33266662670479</v>
@@ -41324,13 +41318,13 @@
         <v>398.34420691544324</v>
       </c>
       <c r="AH124" s="87">
-        <v>1.4530828879606311E-3</v>
+        <v>1.485866160597324E-3</v>
       </c>
       <c r="AI124" s="87">
-        <v>6.6324555996184562E-3</v>
+        <v>2.8197943823391526E-3</v>
       </c>
       <c r="AJ124" s="87">
-        <v>356.14760066311703</v>
+        <v>356.15138054106171</v>
       </c>
       <c r="AK124" s="87">
         <v>7.1613991924958835</v>
@@ -41507,10 +41501,10 @@
         <v>4418.470454693299</v>
       </c>
       <c r="G125" s="87">
-        <v>2493.0038138222553</v>
+        <v>2272.1409795443815</v>
       </c>
       <c r="H125" s="87">
-        <v>3748.3177131521879</v>
+        <v>3969.1805474300618</v>
       </c>
       <c r="I125" s="87">
         <v>997.77190178762191</v>
@@ -41588,13 +41582,13 @@
         <v>1328.6585213024609</v>
       </c>
       <c r="AH125" s="87">
-        <v>4.7491313305657668E-3</v>
+        <v>4.8562773636567679E-3</v>
       </c>
       <c r="AI125" s="87">
-        <v>2.1676948333581757E-2</v>
+        <v>9.2159738153100024E-3</v>
       </c>
       <c r="AJ125" s="87">
-        <v>1164.0022340037387</v>
+        <v>1164.0145878322239</v>
       </c>
       <c r="AK125" s="87">
         <v>672.37186979921614</v>
@@ -41775,10 +41769,10 @@
         <v>11612.668366175927</v>
       </c>
       <c r="G126" s="87">
-        <v>5303.173843492581</v>
+        <v>4833.3494496236162</v>
       </c>
       <c r="H126" s="87">
-        <v>7973.5058339168118</v>
+        <v>8443.3302277857765</v>
       </c>
       <c r="I126" s="87">
         <v>1882.2372086920916</v>
@@ -41856,13 +41850,13 @@
         <v>3777.1320546778193</v>
       </c>
       <c r="AH126" s="87">
-        <v>5.4862258230072751E-3</v>
+        <v>5.6100015817009425E-3</v>
       </c>
       <c r="AI126" s="87">
-        <v>2.50413444973153E-2</v>
+        <v>1.064634982913586E-2</v>
       </c>
       <c r="AJ126" s="87">
-        <v>1344.662564876563</v>
+        <v>1344.6768360954725</v>
       </c>
       <c r="AK126" s="87">
         <v>383.81853776121642</v>
@@ -42043,10 +42037,10 @@
         <v>13987.432478524532</v>
       </c>
       <c r="G127" s="87">
-        <v>9111.6873042735424</v>
+        <v>8304.4550521936198</v>
       </c>
       <c r="H127" s="87">
-        <v>13699.737934595669</v>
+        <v>14506.970186675591</v>
       </c>
       <c r="I127" s="87">
         <v>8487.712189220083</v>
@@ -42124,13 +42118,13 @@
         <v>11846.662409783157</v>
       </c>
       <c r="AH127" s="87">
-        <v>1.2222184940080299E-2</v>
+        <v>1.2497931922187481E-2</v>
       </c>
       <c r="AI127" s="87">
-        <v>5.5786975138891193E-2</v>
+        <v>2.3717881973214981E-2</v>
       </c>
       <c r="AJ127" s="87">
-        <v>2995.6321655743041</v>
+        <v>2995.6639589204874</v>
       </c>
       <c r="AK127" s="87">
         <v>2553.1423345374033</v>
@@ -42311,10 +42305,10 @@
         <v>16222.445084322033</v>
       </c>
       <c r="G128" s="87">
-        <v>33302.69000410047</v>
+        <v>30352.302819531385</v>
       </c>
       <c r="H128" s="87">
-        <v>40520.467297974887</v>
+        <v>43470.854482543975</v>
       </c>
       <c r="I128" s="87">
         <v>19959.593717182455</v>
@@ -42392,13 +42386,13 @@
         <v>7378.9380754579297</v>
       </c>
       <c r="AH128" s="87">
-        <v>6.3816843849269955E-4</v>
+        <v>4.3466803605586697E-2</v>
       </c>
       <c r="AI128" s="87">
-        <v>2.9128578062887129E-3</v>
+        <v>0.24359999999999998</v>
       </c>
       <c r="AJ128" s="87">
-        <v>156.41376029065151</v>
+        <v>156.13024451329071</v>
       </c>
       <c r="AK128" s="87">
         <v>1463.4649484582119</v>
@@ -44965,10 +44959,10 @@
         <v>835.05442659300331</v>
       </c>
       <c r="G143" s="87">
-        <v>332.0817597331</v>
+        <v>302.66162075858909</v>
       </c>
       <c r="H143" s="87">
-        <v>332.0817597331</v>
+        <v>361.50189870761091</v>
       </c>
       <c r="I143" s="87">
         <v>244.85185605166751</v>
@@ -45046,13 +45040,13 @@
         <v>-163.0446890783129</v>
       </c>
       <c r="AH143" s="87">
-        <v>5.9642360641561976E-4</v>
+        <v>4.63463661099483E-4</v>
       </c>
       <c r="AI143" s="87">
-        <v>2.7223175779516069E-3</v>
+        <v>2.1767517831592126E-3</v>
       </c>
       <c r="AJ143" s="87">
-        <v>146.18218790405916</v>
+        <v>146.18286642979928</v>
       </c>
       <c r="AK143" s="87">
         <v>65.757785048502853</v>
@@ -45681,10 +45675,10 @@
         <v>1042.0646315784118</v>
       </c>
       <c r="BK146" s="87">
-        <v>722.09366612754866</v>
+        <v>721.89802218532168</v>
       </c>
       <c r="BL146" s="87">
-        <v>939.88723033003998</v>
+        <v>940.08287427226696</v>
       </c>
       <c r="BM146" s="87">
         <v>5053.493257097075</v>
@@ -45881,10 +45875,10 @@
         <v>-3359.7453508653507</v>
       </c>
       <c r="G147" s="87">
-        <v>-8634.3571129291413</v>
+        <v>-1766.8129644249793</v>
       </c>
       <c r="H147" s="87">
-        <v>-953.44718626286249</v>
+        <v>-1958.381284634449</v>
       </c>
       <c r="I147" s="87">
         <v>-403.85060421393837</v>
@@ -45953,7 +45947,7 @@
         <v>180.89817884259264</v>
       </c>
       <c r="AE147" s="87">
-        <v>-4367.9739710249323</v>
+        <v>-10230.584021157507</v>
       </c>
       <c r="AF147" s="87">
         <v>22.914449623453038</v>
@@ -45962,13 +45956,13 @@
         <v>-371.04312537281521</v>
       </c>
       <c r="AH147" s="87">
-        <v>-8.2741771904378133E-4</v>
+        <v>-6.4296255413369137E-4</v>
       </c>
       <c r="AI147" s="87">
-        <v>-3.7766677519666322E-3</v>
+        <v>-3.0198050110226337E-3</v>
       </c>
       <c r="AJ147" s="87">
-        <v>-202.79836563503486</v>
+        <v>-202.7993069529407</v>
       </c>
       <c r="AK147" s="87">
         <v>-66.835358856716184</v>
@@ -46390,13 +46384,13 @@
         <v>-90.744621482819468</v>
       </c>
       <c r="AH149" s="87">
-        <v>-2.0302184662270785E-4</v>
+        <v>-1.5776244821095949E-4</v>
       </c>
       <c r="AI149" s="87">
-        <v>-9.2667348479169489E-4</v>
+        <v>-7.4096357337723542E-4</v>
       </c>
       <c r="AJ149" s="87">
-        <v>-49.76023317767131</v>
+        <v>-49.760464146981136</v>
       </c>
       <c r="AK149" s="87">
         <v>-12.568338505345672</v>
@@ -47359,10 +47353,10 @@
         <v>80856.433778936684</v>
       </c>
       <c r="G154" s="87">
-        <v>98199.69575640859</v>
+        <v>89476.206652745168</v>
       </c>
       <c r="H154" s="87">
-        <v>127818.09949769097</v>
+        <v>136541.58860135439</v>
       </c>
       <c r="I154" s="87">
         <v>58940.818114347952</v>
@@ -47431,7 +47425,7 @@
         <v>138654.32297346054</v>
       </c>
       <c r="AE154" s="87">
-        <v>58353.212225623225</v>
+        <v>58353.21222562324</v>
       </c>
       <c r="AF154" s="87">
         <v>86484.671755975025</v>
@@ -47446,7 +47440,7 @@
         <v>1</v>
       </c>
       <c r="AJ154" s="87">
-        <v>53697.698403375354</v>
+        <v>53697.698403375383</v>
       </c>
       <c r="AK154" s="87">
         <v>36473.691071377209</v>
@@ -47527,10 +47521,10 @@
         <v>61794.139270354732</v>
       </c>
       <c r="BK154" s="87">
-        <v>99018.313672292163</v>
+        <v>90294.602772421742</v>
       </c>
       <c r="BL154" s="87">
-        <v>195485.60752324775</v>
+        <v>204209.31842311818</v>
       </c>
       <c r="BM154" s="87">
         <v>121063.83472564709</v>
@@ -47795,6 +47789,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:AA67"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -51335,12 +51330,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:AJ101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D21" sqref="D21"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51866,7 +51862,7 @@
         <v>0.74</v>
       </c>
       <c r="C16" s="72">
-        <v>0.74</v>
+        <v>0.39</v>
       </c>
       <c r="D16" s="11">
         <f t="shared" si="1"/>
@@ -51909,10 +51905,10 @@
         <v>cngas</v>
       </c>
       <c r="B17" s="72">
-        <v>0.74</v>
+        <v>1.3</v>
       </c>
       <c r="C17" s="72">
-        <v>0.74</v>
+        <v>0.39</v>
       </c>
       <c r="D17" s="11">
         <f t="shared" si="1"/>
@@ -51956,7 +51952,7 @@
         <v>0.74</v>
       </c>
       <c r="C18" s="72">
-        <v>0.74</v>
+        <v>0.39</v>
       </c>
       <c r="D18" s="11">
         <f t="shared" si="1"/>
@@ -54122,6 +54118,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:AA66"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -56397,6 +56394,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:AO82"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">

</xml_diff>

<commit_message>
Changes in CGE that were left out in previous commit - still pre fcel
</commit_message>
<xml_diff>
--- a/CGE/1model.xlsx
+++ b/CGE/1model.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA3D9CF-5891-4EF1-BB7B-DCB1D4E7BEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6BCF06-548A-439A-BE84-26165B595599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="905" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51336,7 +51336,7 @@
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D21" sqref="D21"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53053,9 +53053,8 @@
         <f>VLOOKUP(VLOOKUP($A42,Elasticities_RawData!$N$8:$O$66,2,),Elasticities_RawData!$E$8:$G$48,2,)</f>
         <v>0.88600000000000001</v>
       </c>
-      <c r="C42" s="22">
-        <f>VLOOKUP(VLOOKUP($A42,Elasticities_RawData!$N$8:$O$66,2,),Elasticities_RawData!$E$8:$G$48,2,)</f>
-        <v>0.88600000000000001</v>
+      <c r="C42" s="72">
+        <v>1.27</v>
       </c>
       <c r="D42" s="11">
         <f t="shared" si="1"/>

</xml_diff>